<commit_message>
Update H2 name in reporting sets
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr backupFile="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E332CD-8857-4FF5-9ADC-8731981B702F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D35EC4-CCEA-47D4-8FFE-BD254709E956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="16" r:id="rId1"/>
@@ -1710,9 +1710,6 @@
     <t>*HET*</t>
   </si>
   <si>
-    <t>SUPH2*</t>
-  </si>
-  <si>
     <t>SEAI_HYDROGEN</t>
   </si>
   <si>
@@ -2056,6 +2053,9 @@
   </si>
   <si>
     <t>Olexandr Balyk (UCC, olexandr.balyk@ucc.ie)</t>
+  </si>
+  <si>
+    <t>H2*</t>
   </si>
 </sst>
 </file>
@@ -2875,7 +2875,7 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -3400,10 +3400,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -3432,10 +3432,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -3464,10 +3464,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -3524,10 +3524,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -3612,10 +3612,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -3700,7 +3700,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B29" s="13">
         <v>1</v>
@@ -3732,10 +3732,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>640</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>641</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -3764,10 +3764,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>642</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>643</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -3797,7 +3797,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="16" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -5785,16 +5785,16 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -5811,16 +5811,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -5837,16 +5837,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -5863,16 +5863,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -5889,16 +5889,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E7" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F7" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -5915,16 +5915,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F8" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G8" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
@@ -5941,16 +5941,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E9" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
@@ -5967,16 +5967,16 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E10" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F10" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G10" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -5993,16 +5993,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E11" t="s">
+        <v>572</v>
+      </c>
+      <c r="F11" t="s">
         <v>573</v>
       </c>
-      <c r="F11" t="s">
-        <v>574</v>
-      </c>
       <c r="G11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -6019,16 +6019,16 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E12" t="s">
+        <v>574</v>
+      </c>
+      <c r="F12" t="s">
         <v>575</v>
       </c>
-      <c r="F12" t="s">
-        <v>576</v>
-      </c>
       <c r="G12" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
@@ -6048,16 +6048,16 @@
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E13" t="s">
+        <v>589</v>
+      </c>
+      <c r="F13" t="s">
+        <v>592</v>
+      </c>
+      <c r="G13" t="s">
         <v>590</v>
-      </c>
-      <c r="F13" t="s">
-        <v>593</v>
-      </c>
-      <c r="G13" t="s">
-        <v>591</v>
       </c>
       <c r="H13" t="s">
         <v>15</v>
@@ -6077,16 +6077,16 @@
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E14" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F14" t="s">
+        <v>593</v>
+      </c>
+      <c r="G14" t="s">
         <v>594</v>
-      </c>
-      <c r="G14" t="s">
-        <v>595</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -6106,16 +6106,16 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E15" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F15" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G15" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -6135,16 +6135,16 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E16" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F16" t="s">
+        <v>598</v>
+      </c>
+      <c r="G16" t="s">
         <v>599</v>
-      </c>
-      <c r="G16" t="s">
-        <v>600</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -6161,16 +6161,16 @@
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D17" t="s">
+        <v>602</v>
+      </c>
+      <c r="F17" t="s">
+        <v>601</v>
+      </c>
+      <c r="G17" t="s">
         <v>603</v>
-      </c>
-      <c r="F17" t="s">
-        <v>602</v>
-      </c>
-      <c r="G17" t="s">
-        <v>604</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -6187,16 +6187,16 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>605</v>
+      </c>
+      <c r="D18" t="s">
+        <v>604</v>
+      </c>
+      <c r="F18" t="s">
         <v>606</v>
       </c>
-      <c r="D18" t="s">
-        <v>605</v>
-      </c>
-      <c r="F18" t="s">
-        <v>607</v>
-      </c>
       <c r="G18" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -6213,16 +6213,16 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>607</v>
+      </c>
+      <c r="D19" t="s">
+        <v>604</v>
+      </c>
+      <c r="F19" t="s">
         <v>608</v>
       </c>
-      <c r="D19" t="s">
-        <v>605</v>
-      </c>
-      <c r="F19" t="s">
-        <v>609</v>
-      </c>
       <c r="G19" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -6249,8 +6249,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6327,7 +6327,7 @@
         <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D4" t="s">
         <v>459</v>
@@ -6483,7 +6483,7 @@
         <v>137</v>
       </c>
       <c r="B10" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D10" t="s">
         <v>460</v>
@@ -6587,7 +6587,7 @@
         <v>137</v>
       </c>
       <c r="B14" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D14" t="s">
         <v>250</v>
@@ -6691,7 +6691,7 @@
         <v>137</v>
       </c>
       <c r="B18" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D18" t="s">
         <v>461</v>
@@ -6795,7 +6795,7 @@
         <v>137</v>
       </c>
       <c r="B22" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D22" t="s">
         <v>257</v>
@@ -6899,7 +6899,7 @@
         <v>137</v>
       </c>
       <c r="B26" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D26" t="s">
         <v>462</v>
@@ -7003,7 +7003,7 @@
         <v>137</v>
       </c>
       <c r="B30" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D30" t="s">
         <v>264</v>
@@ -7107,7 +7107,7 @@
         <v>137</v>
       </c>
       <c r="B34" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D34" t="s">
         <v>463</v>
@@ -7211,7 +7211,7 @@
         <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D38" t="s">
         <v>271</v>
@@ -7315,7 +7315,7 @@
         <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D42" t="s">
         <v>464</v>
@@ -7419,7 +7419,7 @@
         <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D46" t="s">
         <v>278</v>
@@ -7523,7 +7523,7 @@
         <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D50" t="s">
         <v>465</v>
@@ -7627,7 +7627,7 @@
         <v>137</v>
       </c>
       <c r="B54" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D54" t="s">
         <v>285</v>
@@ -7731,7 +7731,7 @@
         <v>137</v>
       </c>
       <c r="B58" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D58" t="s">
         <v>466</v>
@@ -7835,7 +7835,7 @@
         <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D62" t="s">
         <v>292</v>
@@ -7965,7 +7965,7 @@
         <v>163</v>
       </c>
       <c r="B67" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D67" t="s">
         <v>467</v>
@@ -8147,7 +8147,7 @@
         <v>163</v>
       </c>
       <c r="B74" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D74" t="s">
         <v>522</v>
@@ -8173,13 +8173,13 @@
         <v>163</v>
       </c>
       <c r="B75" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D75" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E75" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F75" t="s">
         <v>15</v>
@@ -8199,13 +8199,13 @@
         <v>163</v>
       </c>
       <c r="B76" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D76" t="s">
+        <v>539</v>
+      </c>
+      <c r="E76" t="s">
         <v>540</v>
-      </c>
-      <c r="E76" t="s">
-        <v>541</v>
       </c>
       <c r="F76" t="s">
         <v>15</v>
@@ -8277,13 +8277,13 @@
         <v>163</v>
       </c>
       <c r="B79" t="s">
+        <v>648</v>
+      </c>
+      <c r="D79" t="s">
         <v>533</v>
       </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>534</v>
-      </c>
-      <c r="E79" t="s">
-        <v>535</v>
       </c>
       <c r="F79" t="s">
         <v>15</v>
@@ -8492,7 +8492,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F8" t="s">
         <v>457</v>
@@ -8630,13 +8630,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F14" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G14" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -8653,13 +8653,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F15" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G15" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -8679,13 +8679,13 @@
         <v>325</v>
       </c>
       <c r="B16" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F16" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G16" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -8702,13 +8702,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G17" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -8725,13 +8725,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G18" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
@@ -8748,13 +8748,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F19" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G19" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -8774,13 +8774,13 @@
         <v>325</v>
       </c>
       <c r="B20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F20" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G20" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H20" t="s">
         <v>15</v>
@@ -10913,7 +10913,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11371,7 +11371,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:K3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add H2 and electricity storage sets
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D35EC4-CCEA-47D4-8FFE-BD254709E956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30011893-46ED-4281-BBCF-BACA542A2561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="16" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="655">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -2056,6 +2056,24 @@
   </si>
   <si>
     <t>H2*</t>
+  </si>
+  <si>
+    <t>ELCC</t>
+  </si>
+  <si>
+    <t>STG_ELCC</t>
+  </si>
+  <si>
+    <t>All ELCC storage</t>
+  </si>
+  <si>
+    <t>All H2 storage</t>
+  </si>
+  <si>
+    <t>STG_H2</t>
+  </si>
+  <si>
+    <t>STS</t>
   </si>
 </sst>
 </file>
@@ -6249,8 +6267,8 @@
   </sheetPr>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8308,10 +8326,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8792,6 +8810,58 @@
         <v>15</v>
       </c>
       <c r="K20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>654</v>
+      </c>
+      <c r="D21" t="s">
+        <v>649</v>
+      </c>
+      <c r="F21" t="s">
+        <v>650</v>
+      </c>
+      <c r="G21" t="s">
+        <v>651</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>654</v>
+      </c>
+      <c r="D22" t="s">
+        <v>648</v>
+      </c>
+      <c r="F22" t="s">
+        <v>653</v>
+      </c>
+      <c r="G22" t="s">
+        <v>652</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correct storage input data and enable vintage tracking
</commit_message>
<xml_diff>
--- a/SetRules.xlsx
+++ b/SetRules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30011893-46ED-4281-BBCF-BACA542A2561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA279DD-5AA3-403A-A287-9A7A799CF3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{69765015-6AAF-4B94-8956-691CCC759B47}"/>
   </bookViews>
@@ -2073,7 +2073,7 @@
     <t>STG_H2</t>
   </si>
   <si>
-    <t>STS</t>
+    <t>STS,STG</t>
   </si>
 </sst>
 </file>
@@ -8329,7 +8329,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>